<commit_message>
Corrección nombre columna df jornada actual
</commit_message>
<xml_diff>
--- a/data/jornada_6_inicial.xlsx
+++ b/data/jornada_6_inicial.xlsx
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>RTDO_L</t>
+          <t>RTDO L</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -451,7 +451,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>RTDO_VISITANTE</t>
+          <t>RTDO V</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -461,7 +461,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>RTDO_L.1</t>
+          <t>RTDO L.1</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -476,7 +476,7 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>RTDO_V.1</t>
+          <t>RTDO V.1</t>
         </is>
       </c>
     </row>

</xml_diff>